<commit_message>
Now have working env
</commit_message>
<xml_diff>
--- a/utils/saf_values_female_redone.xlsx
+++ b/utils/saf_values_female_redone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan\Documents\RedMarrowSfactor\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F594375-EDEF-4B6E-B097-56B151A690BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22D3665-A4DA-4139-9C52-1DC469B98FEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="600" windowWidth="19440" windowHeight="15150" firstSheet="9" activeTab="13" xr2:uid="{669EEAF4-1825-45DC-B493-E84CD2F0D0FF}"/>
+    <workbookView xWindow="-28920" yWindow="165" windowWidth="29040" windowHeight="15990" xr2:uid="{669EEAF4-1825-45DC-B493-E84CD2F0D0FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tissue-AM-Masses" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sacrum" sheetId="12" r:id="rId7"/>
     <sheet name="Clavicles" sheetId="6" r:id="rId8"/>
     <sheet name="LumbarVertebrae" sheetId="11" r:id="rId9"/>
-    <sheet name="ThoracaicVertebrae" sheetId="10" r:id="rId10"/>
+    <sheet name="ThoraicVertebrae" sheetId="10" r:id="rId10"/>
     <sheet name="CervicalVertebrae" sheetId="9" r:id="rId11"/>
     <sheet name="Ribs" sheetId="8" r:id="rId12"/>
     <sheet name="Sternum" sheetId="7" r:id="rId13"/>
@@ -162,9 +162,6 @@
     <t>LumbarVertebrae</t>
   </si>
   <si>
-    <t>ThoracaicVertebrae</t>
-  </si>
-  <si>
     <t>CervicalVertebrae</t>
   </si>
   <si>
@@ -218,13 +215,16 @@
   <si>
     <t>TBV-fraction</t>
   </si>
+  <si>
+    <t>ThoraicVertebrae</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -259,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAE66AC4-918F-4755-BB76-C15479E2FB4B}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +591,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>27</v>
@@ -606,13 +606,13 @@
         <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>7.7</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>29.5</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B9">
         <v>112.2</v>
@@ -917,10 +917,10 @@
         <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -937,10 +937,10 @@
         <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -957,10 +957,10 @@
         <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -977,10 +977,10 @@
         <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -997,10 +997,10 @@
         <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1017,10 +1017,10 @@
         <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1037,10 +1037,10 @@
         <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1057,10 +1057,10 @@
         <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1077,10 +1077,10 @@
         <v>32</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1097,10 +1097,10 @@
         <v>32</v>
       </c>
       <c r="F23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1141,10 +1141,10 @@
         <v>32</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1161,10 +1161,10 @@
         <v>32</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1181,10 +1181,10 @@
         <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1201,10 +1201,10 @@
         <v>32</v>
       </c>
       <c r="F28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1221,10 +1221,10 @@
         <v>32</v>
       </c>
       <c r="F29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1241,10 +1241,10 @@
         <v>32</v>
       </c>
       <c r="F30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1261,10 +1261,10 @@
         <v>32</v>
       </c>
       <c r="F31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1281,10 +1281,10 @@
         <v>32</v>
       </c>
       <c r="F32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1301,10 +1301,10 @@
         <v>32</v>
       </c>
       <c r="F33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1321,10 +1321,10 @@
         <v>32</v>
       </c>
       <c r="F34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1341,10 +1341,10 @@
         <v>32</v>
       </c>
       <c r="F35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1371,37 +1371,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -2973,37 +2973,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -4577,37 +4577,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -6181,37 +6181,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -7774,7 +7774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56FFEC2-8655-4577-8981-25BB1B65C58D}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -7785,37 +7785,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -9091,37 +9091,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -10693,37 +10693,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -12297,37 +12297,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -13901,37 +13901,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -15505,37 +15505,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -17109,37 +17109,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -18711,37 +18711,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -20315,37 +20315,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>